<commit_message>
v1.3 Registration test cases update after review
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2FF12E-9BA5-468C-B481-C0089B98D632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Version History" sheetId="1" r:id="rId1"/>
-    <sheet name="LH-TC-REGISTERATION-Reviews" sheetId="2" r:id="rId2"/>
+    <sheet name="LH-TC-REGISTERATION-Reviews" sheetId="2" r:id="rId1"/>
+    <sheet name="Version History" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>Author</t>
   </si>
@@ -73,9 +77,6 @@
   </si>
   <si>
     <t>Mahmoud abdelmageed</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>Review ID</t>
@@ -173,12 +174,27 @@
   </si>
   <si>
     <t>this test case have the same title of the TC_REG_004</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>NotApplicable</t>
+  </si>
+  <si>
+    <t>v1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omar Sherif </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registerations test cases update after review </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -284,48 +300,18 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
         <vertical style="thin">
           <color indexed="64"/>
         </vertical>
@@ -351,7 +337,9 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -616,11 +604,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -651,6 +638,35 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
@@ -685,34 +701,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <tableColumns count="4">
-    <tableColumn id="1" name="Version Number" dataDxfId="15"/>
-    <tableColumn id="2" name="Author" dataDxfId="14"/>
-    <tableColumn id="3" name="Updated Section" dataDxfId="13"/>
-    <tableColumn id="4" name="Date" dataDxfId="12">
-      <calculatedColumnFormula>DATE(2025,4,16)</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J6" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="9">
+      <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J6" totalsRowShown="0" headerRowDxfId="1" dataDxfId="11">
-  <tableColumns count="10">
-    <tableColumn id="1" name="Date" dataDxfId="0">
-      <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="12">
+      <calculatedColumnFormula>DATE(2025,4,16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Review ID" dataDxfId="10"/>
-    <tableColumn id="2" name="Reviewed Entity" dataDxfId="9"/>
-    <tableColumn id="3" name="Reviewer" dataDxfId="8"/>
-    <tableColumn id="4" name="Version" dataDxfId="7"/>
-    <tableColumn id="5" name="Review Comments" dataDxfId="6"/>
-    <tableColumn id="6" name="Actions" dataDxfId="5"/>
-    <tableColumn id="7" name="Owner" dataDxfId="4"/>
-    <tableColumn id="8" name="Owner Status" dataDxfId="3"/>
-    <tableColumn id="9" name="Reviewer verification" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1007,116 +1023,235 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="B1" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17" style="5" customWidth="1"/>
+    <col min="6" max="6" width="39.88671875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="47.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4">
-        <f t="shared" ref="D2" si="0">DATE(2025,4,16)</f>
-        <v>45763</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="11" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <f ca="1">TODAY()</f>
+        <v>45768</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4">
-        <v>45765</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="4">
-        <v>45766</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
+      <c r="C2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="1:10" s="11" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <f t="shared" ref="A3:A6" ca="1" si="0">TODAY()</f>
+        <v>45768</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>45768</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>45768</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.4">
+      <c r="A6" s="8">
+        <f t="shared" ca="1" si="0"/>
+        <v>45768</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+      <formula1>"open,inProgress,notApplicable,close"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I6" xr:uid="{00000000-0002-0000-0100-000001000000}">
+      <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J6" xr:uid="{00000000-0002-0000-0100-000002000000}">
+      <formula1>"Open,Closed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1125,228 +1260,118 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="17" style="5" customWidth="1"/>
-    <col min="6" max="6" width="39.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="47.28515625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4">
+        <f t="shared" ref="D2" si="0">DATE(2025,4,16)</f>
+        <v>45763</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="11" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <f ca="1">TODAY()</f>
-        <v>45767</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="9"/>
-    </row>
-    <row r="3" spans="1:10" s="11" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <f t="shared" ref="A3:A6" ca="1" si="0">TODAY()</f>
-        <v>45767</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
-        <f t="shared" ca="1" si="0"/>
-        <v>45767</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8">
-        <f t="shared" ca="1" si="0"/>
-        <v>45767</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.35">
-      <c r="A6" s="8">
-        <f t="shared" ca="1" si="0"/>
-        <v>45767</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="7"/>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4">
+        <v>45765</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45766</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="4">
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H1048576">
-      <formula1>"open,inProgress,notApplicable,close"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I6">
-      <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J6">
-      <formula1>"Open,Closed"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
v1.0 Registerations test cases update after review
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2FF12E-9BA5-468C-B481-C0089B98D632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59A170D-DA1F-43C4-AFC7-10888EAFDA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Author</t>
   </si>
@@ -46,9 +46,6 @@
     <t>v1.0</t>
   </si>
   <si>
-    <t>intial version</t>
-  </si>
-  <si>
     <t>Version Number</t>
   </si>
   <si>
@@ -76,25 +73,10 @@
     <t>Reviewer verification</t>
   </si>
   <si>
-    <t>Mahmoud abdelmageed</t>
-  </si>
-  <si>
     <t>Review ID</t>
   </si>
   <si>
     <t>Reviewed Entity</t>
-  </si>
-  <si>
-    <t>v1.1</t>
-  </si>
-  <si>
-    <t>v1.2</t>
-  </si>
-  <si>
-    <t>Added reviews for the new version of the Testcases file</t>
-  </si>
-  <si>
-    <t>Added crucial missing review points regarding the TC_ID column and modified Filename review and Status and Actual result column</t>
   </si>
   <si>
     <t>LH_TC_REGITERATION_REVIEW_001</t>
@@ -180,9 +162,6 @@
   </si>
   <si>
     <t>NotApplicable</t>
-  </si>
-  <si>
-    <t>v1.3</t>
   </si>
   <si>
     <t xml:space="preserve">Omar Sherif </t>
@@ -289,6 +268,25 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -668,25 +666,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -701,32 +680,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J6" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J6" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="15">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="0">
       <calculatedColumnFormula>DATE(2025,4,16)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1057,185 +1036,185 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="11" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45768</v>
+        <v>45769</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" s="11" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <f t="shared" ref="A3:A6" ca="1" si="0">TODAY()</f>
-        <v>45768</v>
+        <v>45769</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45768</v>
+        <v>45769</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45768</v>
+        <v>45769</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.4">
       <c r="A6" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>45768</v>
+        <v>45769</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J6" s="7"/>
     </row>
@@ -1264,7 +1243,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1277,13 +1256,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1294,57 +1273,26 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2" si="0">DATE(2025,4,16)</f>
-        <v>45763</v>
+        <v>45768</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="4">
-        <v>45765</v>
-      </c>
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="4">
-        <v>45766</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="4">
-        <v>45768</v>
-      </c>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>

</xml_diff>

<commit_message>
V1.2 close the registration feature review
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59A170D-DA1F-43C4-AFC7-10888EAFDA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH-TC-REGISTERATION-Reviews" sheetId="2" r:id="rId1"/>
     <sheet name="Version History" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>Author</t>
   </si>
@@ -115,13 +109,7 @@
     <t>SRS_ID</t>
   </si>
   <si>
-    <t>V1.1</t>
-  </si>
-  <si>
     <t>V1.2</t>
-  </si>
-  <si>
-    <t>V1.3</t>
   </si>
   <si>
     <t>TC-REG-001</t>
@@ -164,16 +152,26 @@
     <t>NotApplicable</t>
   </si>
   <si>
-    <t xml:space="preserve">Omar Sherif </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registerations test cases update after review </t>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>intial review for the registeration feature</t>
+  </si>
+  <si>
+    <t>update owner status for the reviews</t>
+  </si>
+  <si>
+    <t>Verfiy thu updates
+close the review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omar </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -680,32 +678,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J6" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J6" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="15">
+    <tableColumn id="1" name="Date" dataDxfId="15">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="6"/>
+    <tableColumn id="11" name="Review ID" dataDxfId="14"/>
+    <tableColumn id="2" name="Reviewed Entity" dataDxfId="13"/>
+    <tableColumn id="3" name="Reviewer" dataDxfId="12"/>
+    <tableColumn id="4" name="Version" dataDxfId="11"/>
+    <tableColumn id="5" name="Review Comments" dataDxfId="10"/>
+    <tableColumn id="6" name="Actions" dataDxfId="9"/>
+    <tableColumn id="7" name="Owner" dataDxfId="8"/>
+    <tableColumn id="8" name="Owner Status" dataDxfId="7"/>
+    <tableColumn id="9" name="Reviewer verification" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="0">
+    <tableColumn id="1" name="Version Number" dataDxfId="3"/>
+    <tableColumn id="2" name="Author" dataDxfId="2"/>
+    <tableColumn id="3" name="Updated Section" dataDxfId="1"/>
+    <tableColumn id="4" name="Date" dataDxfId="0">
       <calculatedColumnFormula>DATE(2025,4,16)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1002,36 +1000,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.88671875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="17" style="5" customWidth="1"/>
-    <col min="6" max="6" width="39.88671875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="47.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="20.5546875" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="5"/>
+    <col min="6" max="6" width="39.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="47.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1063,7 +1061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="11" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="11" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
         <v>45769</v>
@@ -1081,20 +1079,22 @@
         <v>17</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="9"/>
+        <v>39</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" s="11" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="11" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <f t="shared" ref="A3:A6" ca="1" si="0">TODAY()</f>
         <v>45769</v>
@@ -1121,11 +1121,13 @@
         <v>19</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <f t="shared" ca="1" si="0"/>
         <v>45769</v>
@@ -1134,29 +1136,31 @@
         <v>22</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <f t="shared" ca="1" si="0"/>
         <v>45769</v>
@@ -1165,29 +1169,31 @@
         <v>23</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A6" s="8">
         <f t="shared" ca="1" si="0"/>
         <v>45769</v>
@@ -1196,38 +1202,40 @@
         <v>24</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="7"/>
+        <v>38</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H1048576">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I6" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I6">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J6" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J6">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1239,22 +1247,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1268,51 +1276,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="4">
+        <v>45767</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D3" s="4">
+        <v>45769</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="4">
-        <v>45768</v>
+      <c r="D4" s="4">
+        <v>45769</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>

</xml_diff>

<commit_message>
v2.0 review the new version of registration TC
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\TCS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="LH-TC-REGISTERATION-Reviews" sheetId="2" r:id="rId1"/>
     <sheet name="Version History" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
   <si>
     <t>Author</t>
   </si>
@@ -115,64 +120,120 @@
     <t>TC-REG-001</t>
   </si>
   <si>
-    <t xml:space="preserve">At the test steps the word "valid email","valid user name"and "valid password" are too vauge </t>
-  </si>
-  <si>
-    <t xml:space="preserve">please mention the conditions of the valid email and the valid passowrd and the valid user name </t>
-  </si>
-  <si>
     <t>there is no test cases for the first SRS in the SRS sheet</t>
   </si>
   <si>
-    <t>please confirm that test cases cover the SRS for the registeration feature</t>
-  </si>
-  <si>
     <t>TC-REG-004</t>
   </si>
   <si>
     <t>TC-REG-005</t>
   </si>
   <si>
-    <t xml:space="preserve">The test case title is not specified, the test case should check one condition numbers or special charachters.
+    <t>specify the title for numbers</t>
+  </si>
+  <si>
+    <t>this test case have the same title of the TC_REG_004</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>update owner status for the reviews</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omar </t>
+  </si>
+  <si>
+    <t>21/4/2025</t>
+  </si>
+  <si>
+    <t>13/5/2025</t>
+  </si>
+  <si>
+    <t>LH-TC-REGISTERATION-016</t>
+  </si>
+  <si>
+    <t>LH_TC_REGITERATION_REVIEW_007</t>
+  </si>
+  <si>
+    <t>Ahmed Abuzaid</t>
+  </si>
+  <si>
+    <t>please the error message in the SRS
+"invalid data"</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>LH_TC_REGITERATION_REVIEW_008</t>
+  </si>
+  <si>
+    <t>LH-TC-REGISTERATION-017</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>LH_TC_REGITERATION_REVIEW_009</t>
+  </si>
+  <si>
+    <t>LH-TC-REGISTERATION.xlsx</t>
+  </si>
+  <si>
+    <t>it must be v2.0 because there is a major change</t>
+  </si>
+  <si>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t>review the new version of registration
+test cases</t>
+  </si>
+  <si>
+    <t>initial review for the registration feature</t>
+  </si>
+  <si>
+    <t>Verify thu updates
+close the review</t>
+  </si>
+  <si>
+    <t>please confirm that test cases cover the SRS for the registration feature</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the test steps the word "valid email","valid user name"and "valid password" are too vague </t>
+  </si>
+  <si>
+    <t xml:space="preserve">please mention the conditions of the valid email and the valid password and the valid user name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The test case title is not specified, the test case should check one condition numbers or special characters.
 </t>
   </si>
   <si>
-    <t>specify the title for numbers</t>
-  </si>
-  <si>
-    <t>specify the title for special charchters</t>
-  </si>
-  <si>
-    <t>this test case have the same title of the TC_REG_004</t>
-  </si>
-  <si>
-    <t>Closed</t>
-  </si>
-  <si>
-    <t>NotApplicable</t>
-  </si>
-  <si>
-    <t>v1.1</t>
-  </si>
-  <si>
-    <t>intial review for the registeration feature</t>
-  </si>
-  <si>
-    <t>update owner status for the reviews</t>
-  </si>
-  <si>
-    <t>Verfiy thu updates
-close the review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omar </t>
+    <t>specify the title for special characters</t>
+  </si>
+  <si>
+    <t>in the expected result you say that the error message  "Username must be 4-20 characters"</t>
+  </si>
+  <si>
+    <t>in the expected result you say that the error message  "Username must be alphanumeric</t>
+  </si>
+  <si>
+    <t>in version history you write it v1.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +254,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -202,7 +269,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -225,11 +292,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -248,9 +376,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -259,6 +384,33 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,7 +830,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J6" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="10">
     <tableColumn id="1" name="Date" dataDxfId="15">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
@@ -1000,7 +1152,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1008,17 +1160,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="17" style="5" customWidth="1"/>
     <col min="6" max="6" width="39.85546875" style="5" customWidth="1"/>
@@ -1061,187 +1213,281 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="11" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <f ca="1">TODAY()</f>
-        <v>45769</v>
-      </c>
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:10" s="10" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="F2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="11" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <f t="shared" ref="A3:A6" ca="1" si="0">TODAY()</f>
-        <v>45769</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="I2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="10" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>38</v>
+      <c r="I3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
-        <f t="shared" ca="1" si="0"/>
-        <v>45769</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="G4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="84" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8">
-        <f t="shared" ca="1" si="0"/>
-        <v>45769</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="9" t="s">
+      <c r="B7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.35">
-      <c r="A6" s="8">
-        <f t="shared" ca="1" si="0"/>
-        <v>45769</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="9" t="s">
+      <c r="I7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="84" x14ac:dyDescent="0.35">
+      <c r="A8" s="11">
+        <f ca="1">TODAY()</f>
+        <v>45790</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>38</v>
+      <c r="I8" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="42" x14ac:dyDescent="0.35">
+      <c r="A9" s="11">
+        <f ca="1">TODAY()</f>
+        <v>45790</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H1048576">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I9">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J9">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1250,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,7 +1530,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D2" s="4">
         <v>45767</v>
@@ -1292,13 +1538,13 @@
     </row>
     <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D3" s="4">
         <v>45769</v>
@@ -1312,10 +1558,24 @@
         <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D4" s="4">
         <v>45769</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v2.1 review comments closed
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\TCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51424AE-4413-4CC4-90B5-A84330198AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH-TC-REGISTERATION-Reviews" sheetId="2" r:id="rId1"/>
     <sheet name="Version History" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t>Author</t>
   </si>
@@ -166,9 +167,6 @@
 "invalid data"</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>LH_TC_REGITERATION_REVIEW_008</t>
   </si>
   <si>
@@ -227,12 +225,21 @@
   </si>
   <si>
     <t>in version history you write it v1.2</t>
+  </si>
+  <si>
+    <t>v2.1</t>
+  </si>
+  <si>
+    <t>Omar Sherif</t>
+  </si>
+  <si>
+    <t>review comments closed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -830,32 +837,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:J9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="10">
-    <tableColumn id="1" name="Date" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="15">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Review ID" dataDxfId="14"/>
-    <tableColumn id="2" name="Reviewed Entity" dataDxfId="13"/>
-    <tableColumn id="3" name="Reviewer" dataDxfId="12"/>
-    <tableColumn id="4" name="Version" dataDxfId="11"/>
-    <tableColumn id="5" name="Review Comments" dataDxfId="10"/>
-    <tableColumn id="6" name="Actions" dataDxfId="9"/>
-    <tableColumn id="7" name="Owner" dataDxfId="8"/>
-    <tableColumn id="8" name="Owner Status" dataDxfId="7"/>
-    <tableColumn id="9" name="Reviewer verification" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Review ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Reviewed Entity" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Reviewer" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Version" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Review Comments" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Actions" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Owner" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Owner Status" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Reviewer verification" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" name="Version Number" dataDxfId="3"/>
-    <tableColumn id="2" name="Author" dataDxfId="2"/>
-    <tableColumn id="3" name="Updated Section" dataDxfId="1"/>
-    <tableColumn id="4" name="Date" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Version Number" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Author" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Updated Section" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date" dataDxfId="0">
       <calculatedColumnFormula>DATE(2025,4,16)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1159,29 +1166,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="B5" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.88671875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="37.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" style="5" customWidth="1"/>
     <col min="5" max="5" width="17" style="5" customWidth="1"/>
-    <col min="6" max="6" width="39.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="47.28515625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="6" max="6" width="39.88671875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="47.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1213,7 +1220,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="10" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="10" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>37</v>
       </c>
@@ -1233,19 +1240,19 @@
         <v>28</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="10" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="10" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>37</v>
       </c>
@@ -1277,7 +1284,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="9" t="s">
         <v>37</v>
       </c>
@@ -1294,10 +1301,10 @@
         <v>17</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>19</v>
@@ -1309,7 +1316,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.4">
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
@@ -1326,7 +1333,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>31</v>
@@ -1341,7 +1348,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.4">
       <c r="A6" s="9" t="s">
         <v>37</v>
       </c>
@@ -1361,7 +1368,7 @@
         <v>32</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>19</v>
@@ -1373,7 +1380,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="84" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="84" x14ac:dyDescent="0.4">
       <c r="A7" s="13" t="s">
         <v>38</v>
       </c>
@@ -1387,10 +1394,10 @@
         <v>41</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>42</v>
@@ -1399,31 +1406,31 @@
         <v>19</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="84" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="84" x14ac:dyDescent="0.4">
       <c r="A8" s="11">
         <f ca="1">TODAY()</f>
         <v>45790</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>45</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>42</v>
@@ -1432,55 +1439,55 @@
         <v>19</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="42" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="42" x14ac:dyDescent="0.4">
       <c r="A9" s="11">
         <f ca="1">TODAY()</f>
         <v>45790</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>48</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>41</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>19</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I9" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J9" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1493,22 +1500,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1522,7 +1529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1530,13 +1537,13 @@
         <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="4">
         <v>45767</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -1550,7 +1557,7 @@
         <v>45769</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -1558,45 +1565,53 @@
         <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" s="4">
         <v>45769</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>

</xml_diff>

<commit_message>
v2.0 Update some test cases after Review of Ahmed
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51424AE-4413-4CC4-90B5-A84330198AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D353AB5D-3813-42FB-9FAD-2B07C0F4768E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1504,7 +1504,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
v2.1 close reviewer status
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_REGISTRATION_REVIEWS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\TCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D353AB5D-3813-42FB-9FAD-2B07C0F4768E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH-TC-REGISTERATION-Reviews" sheetId="2" r:id="rId1"/>
     <sheet name="Version History" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="64">
   <si>
     <t>Author</t>
   </si>
@@ -230,16 +229,13 @@
     <t>v2.1</t>
   </si>
   <si>
-    <t>Omar Sherif</t>
-  </si>
-  <si>
-    <t>review comments closed</t>
+    <t xml:space="preserve">close reviewer status </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -837,32 +833,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:J9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="15">
+    <tableColumn id="1" name="Date" dataDxfId="15">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Review ID" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Reviewed Entity" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Reviewer" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Version" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Review Comments" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Actions" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Owner" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Owner Status" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Reviewer verification" dataDxfId="6"/>
+    <tableColumn id="11" name="Review ID" dataDxfId="14"/>
+    <tableColumn id="2" name="Reviewed Entity" dataDxfId="13"/>
+    <tableColumn id="3" name="Reviewer" dataDxfId="12"/>
+    <tableColumn id="4" name="Version" dataDxfId="11"/>
+    <tableColumn id="5" name="Review Comments" dataDxfId="10"/>
+    <tableColumn id="6" name="Actions" dataDxfId="9"/>
+    <tableColumn id="7" name="Owner" dataDxfId="8"/>
+    <tableColumn id="8" name="Owner Status" dataDxfId="7"/>
+    <tableColumn id="9" name="Reviewer verification" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Version Number" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Author" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Updated Section" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date" dataDxfId="0">
+    <tableColumn id="1" name="Version Number" dataDxfId="3"/>
+    <tableColumn id="2" name="Author" dataDxfId="2"/>
+    <tableColumn id="3" name="Updated Section" dataDxfId="1"/>
+    <tableColumn id="4" name="Date" dataDxfId="0">
       <calculatedColumnFormula>DATE(2025,4,16)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1166,29 +1162,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView topLeftCell="B5" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.88671875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="37.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="17" style="5" customWidth="1"/>
-    <col min="6" max="6" width="39.88671875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="47.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="20.5546875" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="5"/>
+    <col min="6" max="6" width="39.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="47.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1220,7 +1216,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="10" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="10" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>37</v>
       </c>
@@ -1252,7 +1248,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="10" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="10" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>37</v>
       </c>
@@ -1284,7 +1280,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>37</v>
       </c>
@@ -1316,7 +1312,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
@@ -1348,7 +1344,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>37</v>
       </c>
@@ -1380,7 +1376,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="84" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" ht="84" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>38</v>
       </c>
@@ -1412,7 +1408,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="84" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="84" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <f ca="1">TODAY()</f>
         <v>45790</v>
@@ -1445,7 +1441,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="42" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <f ca="1">TODAY()</f>
         <v>45790</v>
@@ -1481,13 +1477,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H1048576">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I9" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I9">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J9" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J9">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1500,22 +1496,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1529,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1543,7 +1539,7 @@
         <v>45767</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -1557,7 +1553,7 @@
         <v>45769</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -1571,7 +1567,7 @@
         <v>45769</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1585,33 +1581,33 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>62</v>
       </c>
       <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>

</xml_diff>